<commit_message>
Cambios locales en Datos.xlsx antes del merge
</commit_message>
<xml_diff>
--- a/Maxiquiosco/Precarga/Datos.xlsx
+++ b/Maxiquiosco/Precarga/Datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\MaxiquioscoPrograII\Maxiquiosco\Precarga\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\estebanr\Documents\GitHub\MaxiquioscoPrograII\Maxiquiosco\Precarga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAE23426-03A1-4BB5-8124-1DAD85F1FC98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F76118-11B1-4BD2-A81D-67EE99F66A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{8B33AC1D-F671-460C-A3A2-2B7F0EEA1529}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8B33AC1D-F671-460C-A3A2-2B7F0EEA1529}"/>
   </bookViews>
   <sheets>
     <sheet name="Proveedores" sheetId="1" r:id="rId1"/>
@@ -323,7 +323,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -350,7 +350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -699,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2584C2D2-E4C6-4BCF-B375-30D8D80EC49F}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="A1:G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,6 +741,15 @@
       <c r="G1" s="2">
         <v>96094200</v>
       </c>
+      <c r="H1" s="2">
+        <v>96209157</v>
+      </c>
+      <c r="I1" s="2">
+        <v>96757308</v>
+      </c>
+      <c r="J1" s="3">
+        <v>96227218</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
@@ -764,6 +773,15 @@
       <c r="G2" s="5">
         <v>2096094200</v>
       </c>
+      <c r="H2" s="5">
+        <v>2096209157</v>
+      </c>
+      <c r="I2" s="5">
+        <v>2096757308</v>
+      </c>
+      <c r="J2" s="6">
+        <v>2096227218</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -787,6 +805,15 @@
       <c r="G3" s="5">
         <v>1138208671</v>
       </c>
+      <c r="H3" s="5">
+        <v>1137073933</v>
+      </c>
+      <c r="I3" s="5">
+        <v>1139871834</v>
+      </c>
+      <c r="J3" s="6">
+        <v>1136274339</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -810,6 +837,15 @@
       <c r="G4" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="H4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
@@ -833,6 +869,15 @@
       <c r="G5" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="H5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
@@ -856,71 +901,13 @@
       <c r="G6" s="8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H13" s="2">
-        <v>96209157</v>
-      </c>
-      <c r="I13" s="2">
-        <v>96757308</v>
-      </c>
-      <c r="J13" s="3">
-        <v>96227218</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H14" s="5">
-        <v>2096209157</v>
-      </c>
-      <c r="I14" s="5">
-        <v>2096757308</v>
-      </c>
-      <c r="J14" s="6">
-        <v>2096227218</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H15" s="5">
-        <v>1137073933</v>
-      </c>
-      <c r="I15" s="5">
-        <v>1139871834</v>
-      </c>
-      <c r="J15" s="6">
-        <v>1136274339</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="8:10" x14ac:dyDescent="0.25">
-      <c r="H17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="8:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H18" s="8" t="s">
+      <c r="H6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>29</v>
       </c>
     </row>
@@ -934,8 +921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD00DEA7-8A0E-430E-805C-0A49C649D9A5}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>